<commit_message>
add lookup for broader and related
</commit_message>
<xml_diff>
--- a/test_import_pp.xlsx
+++ b/test_import_pp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\Documents\05. RCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\Documents\05. RCE\CHT\cht-poolparty-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3173535-68E8-404C-9EBD-0073774390AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A132B2D1-73BD-4957-8480-6072F9C59D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6E3C263-6518-405E-8427-6ADC26387420}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C6E3C263-6518-405E-8427-6ADC26387420}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>volgnummer</t>
   </si>
   <si>
-    <t>broader term</t>
-  </si>
-  <si>
     <t>broader_uri</t>
   </si>
   <si>
@@ -46,18 +43,12 @@
     <t>alternatief</t>
   </si>
   <si>
-    <t>related</t>
-  </si>
-  <si>
     <t>https://data.cultureelerfgoed.nl/term/id/cht/aa872ce6-a74c-4f81-96ec-6ee0e717f92a</t>
   </si>
   <si>
     <t>testterm</t>
   </si>
   <si>
-    <t>testenterm</t>
-  </si>
-  <si>
     <t>betonwaren</t>
   </si>
   <si>
@@ -155,6 +146,21 @@
   </si>
   <si>
     <t>import test om excel naar ttl import te testen</t>
+  </si>
+  <si>
+    <t>testenterm | alternatief2</t>
+  </si>
+  <si>
+    <t>gerelateerd</t>
+  </si>
+  <si>
+    <t>betonwaren|gaafheid</t>
+  </si>
+  <si>
+    <t>broader_term</t>
+  </si>
+  <si>
+    <t>constructies</t>
   </si>
 </sst>
 </file>
@@ -190,10 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -201,10 +210,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -522,64 +527,64 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -595,247 +600,246 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="5"/>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>